<commit_message>
made mult serch work
make mult search work by funnling it back into search using username single search.

made it so that transfering 0 does not create a history.
</commit_message>
<xml_diff>
--- a/timesForWebsite.xlsx
+++ b/timesForWebsite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\SDN-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD23C0C-3DAF-4566-A9B7-D52A0B2EA5D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320B330F-3464-4433-A190-A42B8F541875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{99A12262-A985-4CC1-A4EE-14DA4F339661}"/>
   </bookViews>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9077FED-0AAF-4BE5-B756-CBB7D566A928}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,6 +437,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43566</v>
+      </c>
+      <c r="B6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43567</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>